<commit_message>
商品藏品信息脚本数据框结构和输出更新【Dataframe Structure and Output Updates in Customized Program 07】
1. 现在，商品藏品信息脚本将将蓝色精粹价格和点券价格分开来。（第468、505、523～531和559行。）
Now, Customized Program 07 will divide the prices into IP and RP prices. (Lines 468, 505, 523～531 and 559.)
2. 现在，商品藏品信息脚本将按照查战绩脚本的套路，输出商品和藏品信息json文件。（第391～394、396和398～401行。）
Now, Customized Program 07 will output the catalog and collection information json files, following the tradition of Customized Program 05. (Lines 391～394, 396 and 398～401.)
3. 跟进第1条更新，更新了自定义脚本主数据框结构工作簿。
Following the first update, updated the Customized Program Main Dataframe Structure workbook.
</commit_message>
<xml_diff>
--- a/Customized Program Main Dataframe Structure.xlsx
+++ b/Customized Program Main Dataframe Structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19250\Documents\GitHub\LoL-DIY-Programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AE6F39-E1D4-4D56-A3CF-2C0F427790FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EBC87F-5074-4463-8423-B56DAF23AB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B2D932DB-2183-440F-AF66-43F3E8354BB0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="6" xr2:uid="{B2D932DB-2183-440F-AF66-43F3E8354BB0}"/>
   </bookViews>
   <sheets>
     <sheet name="05 - mastery_header" sheetId="3" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2270" uniqueCount="940">
   <si>
     <t>gameCreationDate</t>
   </si>
@@ -2811,12 +2811,6 @@
     <t>拥有状态</t>
   </si>
   <si>
-    <t>prices</t>
-  </si>
-  <si>
-    <t>价格</t>
-  </si>
-  <si>
     <t>purchaseData</t>
   </si>
   <si>
@@ -3026,6 +3020,22 @@
   </si>
   <si>
     <t>playerId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>price_IP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>价格（蓝色精粹）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>price_RP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>价格（点券）</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3286,9 +3296,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3326,7 +3336,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3432,7 +3442,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3574,7 +3584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3584,7 +3594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF82C05-E00D-47FE-907F-7796571974D3}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3730,10 +3740,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>931</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>933</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>935</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -3742,10 +3752,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>932</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>934</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>936</v>
       </c>
       <c r="D10" s="7"/>
     </row>
@@ -3786,7 +3796,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>656</v>
@@ -3992,10 +4002,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>149</v>
@@ -4006,10 +4016,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>149</v>
@@ -4023,7 +4033,7 @@
         <v>293</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>149</v>
@@ -4034,10 +4044,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>918</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>920</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>922</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>149</v>
@@ -4051,7 +4061,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="7" t="s">
@@ -4066,7 +4076,7 @@
         <v>292</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>149</v>
@@ -4077,10 +4087,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>149</v>
@@ -4142,10 +4152,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>906</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>908</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>910</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>149</v>
@@ -4189,10 +4199,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23">
@@ -4252,7 +4262,7 @@
         <v>324</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="D27" s="7"/>
     </row>
@@ -6437,10 +6447,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="25" t="s">
+        <v>919</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>921</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>923</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -6578,10 +6588,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="25" t="s">
+        <v>907</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>909</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>911</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -9365,10 +9375,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>149</v>
@@ -9379,10 +9389,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>149</v>
@@ -9410,10 +9420,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>919</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>921</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>923</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>149</v>
@@ -9427,7 +9437,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="7" t="s">
@@ -9518,10 +9528,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>907</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>909</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>911</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>149</v>
@@ -9565,10 +9575,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16">
@@ -12148,10 +12158,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="25" t="s">
+        <v>919</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>921</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -12277,10 +12287,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="25" t="s">
+        <v>907</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>909</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -14289,10 +14299,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="25" t="s">
+        <v>919</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>921</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>923</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -14430,10 +14440,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="25" t="s">
+        <v>907</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>909</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>911</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -16313,9 +16323,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9078C510-49E8-4816-91AD-BE458B8B69FF}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16384,7 +16394,7 @@
         <v>856</v>
       </c>
       <c r="E4">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -16392,7 +16402,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="C5" t="s">
         <v>857</v>
@@ -16494,7 +16504,7 @@
         <v>149</v>
       </c>
       <c r="E11">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -16511,7 +16521,7 @@
         <v>149</v>
       </c>
       <c r="E12">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -16525,7 +16535,7 @@
         <v>871</v>
       </c>
       <c r="E13">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -16533,10 +16543,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>872</v>
+        <v>936</v>
       </c>
       <c r="C14" t="s">
-        <v>873</v>
+        <v>937</v>
       </c>
       <c r="E14">
         <v>11</v>
@@ -16547,13 +16557,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>874</v>
+        <v>938</v>
       </c>
       <c r="C15" t="s">
-        <v>875</v>
+        <v>939</v>
       </c>
       <c r="E15">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -16561,13 +16571,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="C16" t="s">
-        <v>877</v>
-      </c>
-      <c r="D16" t="s">
-        <v>149</v>
+        <v>873</v>
       </c>
       <c r="E16">
         <v>15</v>
@@ -16578,13 +16585,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="C17" t="s">
-        <v>879</v>
+        <v>875</v>
+      </c>
+      <c r="D17" t="s">
+        <v>149</v>
       </c>
       <c r="E17">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -16592,13 +16602,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="C18" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="E18">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -16606,13 +16616,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C19" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -16620,16 +16630,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="C20" t="s">
-        <v>885</v>
-      </c>
-      <c r="D20" t="s">
-        <v>149</v>
+        <v>881</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.2">
@@ -16637,16 +16644,33 @@
         <v>19</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>882</v>
+      </c>
+      <c r="C21" t="s">
+        <v>883</v>
+      </c>
+      <c r="D21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>792</v>
       </c>
-      <c r="C21" t="s">
-        <v>886</v>
-      </c>
-      <c r="D21" t="s">
-        <v>149</v>
-      </c>
-      <c r="E21">
-        <v>18</v>
+      <c r="C22" t="s">
+        <v>884</v>
+      </c>
+      <c r="D22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -16692,10 +16716,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="C2" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -16706,10 +16730,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="C3" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="D3" t="s">
         <v>149</v>
@@ -16754,7 +16778,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="D6" t="s">
         <v>149</v>
@@ -16765,7 +16789,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D7" t="s">
         <v>149</v>
@@ -16796,7 +16820,7 @@
         <v>870</v>
       </c>
       <c r="C9" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -16807,10 +16831,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="C10" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E10">
         <v>9</v>
@@ -16821,10 +16845,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="C11" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="D11" t="s">
         <v>149</v>
@@ -16838,10 +16862,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C12" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="D12" t="s">
         <v>149</v>
@@ -16855,10 +16879,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C13" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="D13" t="s">
         <v>149</v>
@@ -16875,7 +16899,7 @@
         <v>257</v>
       </c>
       <c r="C14" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D14" t="s">
         <v>149</v>
@@ -16889,10 +16913,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="D15" t="s">
         <v>149</v>
@@ -16906,10 +16930,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C16" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="E16">
         <v>0</v>

</xml_diff>